<commit_message>
Got the Icache working and tested.
</commit_message>
<xml_diff>
--- a/doc/MIPS-2-AXP-Conversion.xlsx
+++ b/doc/MIPS-2-AXP-Conversion.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="18195" windowHeight="11070"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="MIPS_to_AXP" localSheetId="0">Sheet1!$A$2:$Z$184</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="523">
   <si>
     <t>0x00000000</t>
   </si>
@@ -1605,13 +1605,16 @@
   </si>
   <si>
     <t>AXP Address</t>
+  </si>
+  <si>
+    <t>0x0000027c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1744,7 +1747,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1894,7 +1907,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1929,7 +1941,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2105,15 +2116,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z180" sqref="Z180"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A185" sqref="A185"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
@@ -2142,7 +2153,7 @@
     <col min="25" max="26" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>252</v>
       </c>
@@ -2208,7 +2219,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2296,11 +2307,11 @@
         <v>0</v>
       </c>
       <c r="Z2" t="str">
-        <f t="shared" ref="Z2:Z54" si="0">IF(ISBLANK(F2),"","0x"&amp;DEC2HEX(Y2+(F2*4)+4,8))</f>
+        <f t="shared" ref="Z2:Z65" si="0">IF(ISBLANK(F2),"","0x"&amp;DEC2HEX(Y2+(F2*4)+4,8))</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -2394,7 +2405,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -2488,7 +2499,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26">
       <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
@@ -2582,7 +2593,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -2676,7 +2687,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -2770,7 +2781,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -2864,7 +2875,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26">
       <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
@@ -2958,7 +2969,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -3052,7 +3063,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26">
       <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
@@ -3146,7 +3157,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
@@ -3240,7 +3251,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26">
       <c r="A13" s="8" t="s">
         <v>26</v>
       </c>
@@ -3334,7 +3345,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -3428,7 +3439,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26">
       <c r="A15" s="5" t="s">
         <v>28</v>
       </c>
@@ -3522,7 +3533,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26">
       <c r="A16" s="5" t="s">
         <v>29</v>
       </c>
@@ -3616,7 +3627,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26">
       <c r="A17" s="8" t="s">
         <v>30</v>
       </c>
@@ -3710,7 +3721,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
@@ -3804,7 +3815,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26">
       <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
@@ -3898,7 +3909,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26">
       <c r="A20" s="5" t="s">
         <v>33</v>
       </c>
@@ -3992,7 +4003,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26">
       <c r="A21" s="8" t="s">
         <v>34</v>
       </c>
@@ -4086,7 +4097,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26">
       <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
@@ -4180,7 +4191,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26">
       <c r="A23" s="5" t="s">
         <v>36</v>
       </c>
@@ -4274,7 +4285,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26">
       <c r="A24" s="5" t="s">
         <v>38</v>
       </c>
@@ -4362,7 +4373,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26">
       <c r="A25" s="8" t="s">
         <v>41</v>
       </c>
@@ -4450,7 +4461,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26">
       <c r="A26" s="1" t="s">
         <v>43</v>
       </c>
@@ -4538,7 +4549,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26">
       <c r="A27" s="5" t="s">
         <v>44</v>
       </c>
@@ -4626,7 +4637,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26">
       <c r="A28" s="5" t="s">
         <v>46</v>
       </c>
@@ -4714,7 +4725,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26">
       <c r="A29" s="8" t="s">
         <v>47</v>
       </c>
@@ -4802,7 +4813,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26">
       <c r="A30" s="1" t="s">
         <v>50</v>
       </c>
@@ -4896,7 +4907,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26">
       <c r="A31" s="5" t="s">
         <v>51</v>
       </c>
@@ -4990,7 +5001,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26">
       <c r="A32" s="5" t="s">
         <v>52</v>
       </c>
@@ -5084,7 +5095,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26">
       <c r="A33" s="8" t="s">
         <v>53</v>
       </c>
@@ -5178,7 +5189,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26">
       <c r="A34" s="1" t="s">
         <v>54</v>
       </c>
@@ -5272,7 +5283,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26">
       <c r="A35" s="5" t="s">
         <v>56</v>
       </c>
@@ -5366,7 +5377,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26">
       <c r="A36" s="5" t="s">
         <v>58</v>
       </c>
@@ -5460,7 +5471,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26">
       <c r="A37" s="8" t="s">
         <v>60</v>
       </c>
@@ -5548,7 +5559,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26">
       <c r="A38" s="1" t="s">
         <v>63</v>
       </c>
@@ -5636,7 +5647,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26">
       <c r="A39" s="5" t="s">
         <v>65</v>
       </c>
@@ -5730,7 +5741,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26">
       <c r="A40" s="5" t="s">
         <v>67</v>
       </c>
@@ -5818,7 +5829,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26">
       <c r="A41" s="8" t="s">
         <v>69</v>
       </c>
@@ -5906,7 +5917,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26">
       <c r="A42" s="1" t="s">
         <v>70</v>
       </c>
@@ -6000,7 +6011,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26">
       <c r="A43" s="5" t="s">
         <v>71</v>
       </c>
@@ -6088,7 +6099,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26">
       <c r="A44" s="5" t="s">
         <v>73</v>
       </c>
@@ -6176,7 +6187,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26">
       <c r="A45" s="8" t="s">
         <v>74</v>
       </c>
@@ -6270,7 +6281,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26">
       <c r="A46" s="1" t="s">
         <v>76</v>
       </c>
@@ -6364,7 +6375,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26">
       <c r="A47" s="5" t="s">
         <v>77</v>
       </c>
@@ -6458,7 +6469,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26">
       <c r="A48" s="5" t="s">
         <v>79</v>
       </c>
@@ -6546,7 +6557,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26">
       <c r="A49" s="8" t="s">
         <v>80</v>
       </c>
@@ -6634,7 +6645,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26">
       <c r="A50" s="1" t="s">
         <v>81</v>
       </c>
@@ -6722,7 +6733,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26">
       <c r="A51" s="5" t="s">
         <v>83</v>
       </c>
@@ -6810,7 +6821,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26">
       <c r="A52" s="5" t="s">
         <v>84</v>
       </c>
@@ -6898,7 +6909,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26">
       <c r="A53" s="8" t="s">
         <v>85</v>
       </c>
@@ -6986,7 +6997,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26">
       <c r="A54" s="1" t="s">
         <v>86</v>
       </c>
@@ -7080,7 +7091,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26">
       <c r="A55" s="5" t="s">
         <v>88</v>
       </c>
@@ -7172,11 +7183,11 @@
         <v>212</v>
       </c>
       <c r="Z55" t="str">
-        <f>IF(ISBLANK(F55),"","0x"&amp;DEC2HEX(Y55+(F55*4)+4,8))</f>
+        <f t="shared" si="0"/>
         <v>0x00000270</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26">
       <c r="A56" s="5" t="s">
         <v>91</v>
       </c>
@@ -7266,11 +7277,11 @@
         <v>216</v>
       </c>
       <c r="Z56" t="str">
-        <f t="shared" ref="Z56:Z119" si="24">IF(ISBLANK(F56),"","0x"&amp;DEC2HEX(Y56+(F56*4)+4,8))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26">
       <c r="A57" s="8" t="s">
         <v>93</v>
       </c>
@@ -7354,11 +7365,11 @@
         <v>220</v>
       </c>
       <c r="Z57" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26">
       <c r="A58" s="1" t="s">
         <v>95</v>
       </c>
@@ -7448,11 +7459,11 @@
         <v>224</v>
       </c>
       <c r="Z58" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26">
       <c r="A59" s="5" t="s">
         <v>97</v>
       </c>
@@ -7542,11 +7553,11 @@
         <v>228</v>
       </c>
       <c r="Z59" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26">
       <c r="A60" s="5" t="s">
         <v>99</v>
       </c>
@@ -7636,11 +7647,11 @@
         <v>232</v>
       </c>
       <c r="Z60" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26">
       <c r="A61" s="8" t="s">
         <v>100</v>
       </c>
@@ -7730,11 +7741,11 @@
         <v>236</v>
       </c>
       <c r="Z61" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26">
       <c r="A62" s="1" t="s">
         <v>257</v>
       </c>
@@ -7767,11 +7778,11 @@
         <v>R22</v>
       </c>
       <c r="K62" s="3" t="str">
-        <f t="shared" ref="K62" si="25">TRIM(MID(I62,FIND(",",I62)+1,LEN(I62)-FIND(",",I62,FIND(",",I62)+1)))</f>
+        <f t="shared" ref="K62" si="24">TRIM(MID(I62,FIND(",",I62)+1,LEN(I62)-FIND(",",I62,FIND(",",I62)+1)))</f>
         <v>R31</v>
       </c>
       <c r="L62" s="3" t="str">
-        <f t="shared" ref="L62" si="26">TRIM(MID(I62,FIND(",",I62,FIND(",",I62)+1)+1,99))</f>
+        <f t="shared" ref="L62" si="25">TRIM(MID(I62,FIND(",",I62,FIND(",",I62)+1)+1,99))</f>
         <v>R22</v>
       </c>
       <c r="M62" s="3" t="str">
@@ -7779,7 +7790,7 @@
         <v>010000</v>
       </c>
       <c r="N62" s="3" t="str">
-        <f t="shared" ref="N62" si="27">DEC2BIN(INT(MID(J62,2,2)),5)</f>
+        <f t="shared" ref="N62" si="26">DEC2BIN(INT(MID(J62,2,2)),5)</f>
         <v>10110</v>
       </c>
       <c r="O62" s="3" t="str">
@@ -7824,11 +7835,11 @@
         <v>240</v>
       </c>
       <c r="Z62" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26">
       <c r="A63" s="5" t="s">
         <v>104</v>
       </c>
@@ -7920,11 +7931,11 @@
         <v>244</v>
       </c>
       <c r="Z63" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="0"/>
         <v>0x00000108</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26">
       <c r="A64" s="5" t="s">
         <v>106</v>
       </c>
@@ -8014,11 +8025,11 @@
         <v>248</v>
       </c>
       <c r="Z64" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26">
       <c r="A65" s="8" t="s">
         <v>107</v>
       </c>
@@ -8108,11 +8119,11 @@
         <v>252</v>
       </c>
       <c r="Z65" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26">
       <c r="A66" s="1" t="s">
         <v>108</v>
       </c>
@@ -8202,11 +8213,11 @@
         <v>256</v>
       </c>
       <c r="Z66" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" ref="Z66:Z129" si="27">IF(ISBLANK(F66),"","0x"&amp;DEC2HEX(Y66+(F66*4)+4,8))</f>
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26">
       <c r="A67" s="5" t="s">
         <v>110</v>
       </c>
@@ -8296,11 +8307,11 @@
         <v>260</v>
       </c>
       <c r="Z67" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26">
       <c r="A68" s="5" t="s">
         <v>112</v>
       </c>
@@ -8392,11 +8403,11 @@
         <v>264</v>
       </c>
       <c r="Z68" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0x000000E8</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26">
       <c r="A69" s="8" t="s">
         <v>113</v>
       </c>
@@ -8480,11 +8491,11 @@
         <v>268</v>
       </c>
       <c r="Z69" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26">
       <c r="A70" s="1" t="s">
         <v>257</v>
       </c>
@@ -8574,11 +8585,11 @@
         <v>272</v>
       </c>
       <c r="Z70" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26">
       <c r="A71" s="5" t="s">
         <v>114</v>
       </c>
@@ -8668,11 +8679,11 @@
         <v>276</v>
       </c>
       <c r="Z71" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26">
       <c r="A72" s="5" t="s">
         <v>116</v>
       </c>
@@ -8762,11 +8773,11 @@
         <v>280</v>
       </c>
       <c r="Z72" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26">
       <c r="A73" s="8" t="s">
         <v>117</v>
       </c>
@@ -8856,11 +8867,11 @@
         <v>284</v>
       </c>
       <c r="Z73" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26">
       <c r="A74" s="1" t="s">
         <v>119</v>
       </c>
@@ -8950,11 +8961,11 @@
         <v>288</v>
       </c>
       <c r="Z74" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26">
       <c r="A75" s="5" t="s">
         <v>121</v>
       </c>
@@ -9044,11 +9055,11 @@
         <v>292</v>
       </c>
       <c r="Z75" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26">
       <c r="A76" s="5" t="s">
         <v>123</v>
       </c>
@@ -9138,11 +9149,11 @@
         <v>296</v>
       </c>
       <c r="Z76" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26">
       <c r="A77" s="8" t="s">
         <v>125</v>
       </c>
@@ -9232,11 +9243,11 @@
         <v>300</v>
       </c>
       <c r="Z77" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26">
       <c r="A78" s="1" t="s">
         <v>127</v>
       </c>
@@ -9320,11 +9331,11 @@
         <v>304</v>
       </c>
       <c r="Z78" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26">
       <c r="A79" s="5" t="s">
         <v>129</v>
       </c>
@@ -9414,11 +9425,11 @@
         <v>308</v>
       </c>
       <c r="Z79" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26">
       <c r="A80" s="5" t="s">
         <v>131</v>
       </c>
@@ -9508,11 +9519,11 @@
         <v>312</v>
       </c>
       <c r="Z80" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26">
       <c r="A81" s="8"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
@@ -9596,11 +9607,11 @@
         <v>316</v>
       </c>
       <c r="Z81" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26">
       <c r="A82" s="1" t="s">
         <v>257</v>
       </c>
@@ -9690,11 +9701,11 @@
         <v>320</v>
       </c>
       <c r="Z82" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26">
       <c r="A83" s="5"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
@@ -9778,11 +9789,11 @@
         <v>324</v>
       </c>
       <c r="Z83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26">
       <c r="A84" s="5" t="s">
         <v>134</v>
       </c>
@@ -9801,8 +9812,8 @@
         <v>0x00000148</v>
       </c>
       <c r="F84" s="16">
-        <f>(D86-D85)/4</f>
-        <v>1</v>
+        <f>(D87-D85)/4</f>
+        <v>2</v>
       </c>
       <c r="G84" s="6" t="s">
         <v>105</v>
@@ -9819,7 +9830,7 @@
       </c>
       <c r="K84" s="7" t="str">
         <f>"0x"&amp;LOWER(IF(MID(DEC2HEX(F84,10),LEN(DEC2HEX(F84,10))-6,1)="F","1","0")&amp;MID(DEC2HEX(F84,10),LEN(DEC2HEX(F84,10))-4,5))</f>
-        <v>0x000001</v>
+        <v>0x000002</v>
       </c>
       <c r="L84" s="7"/>
       <c r="M84" s="7" t="str">
@@ -9832,7 +9843,7 @@
       </c>
       <c r="O84" s="7" t="str">
         <f>"00000"&amp;"00000000"&amp;HEX2BIN(MID(K84,3,99),8)</f>
-        <v>000000000000000000001</v>
+        <v>000000000000000000010</v>
       </c>
       <c r="P84" s="7" t="str">
         <f>IFERROR(HEX2BIN(MID(H84,FIND(".",H84)+1,99),7),"")</f>
@@ -9851,11 +9862,11 @@
       </c>
       <c r="T84" s="7" t="str">
         <f>M84&amp;N84&amp;O84&amp;P84&amp;Q84</f>
-        <v>11110100010000000000000000000001</v>
+        <v>11110100010000000000000000000010</v>
       </c>
       <c r="U84" s="13" t="str">
         <f t="shared" si="47"/>
-        <v>0xf4400001</v>
+        <v>0xf4400002</v>
       </c>
       <c r="V84" s="7">
         <f t="shared" si="38"/>
@@ -9867,18 +9878,18 @@
       </c>
       <c r="X84" t="str">
         <f t="shared" si="40"/>
-        <v>0xf4400001,</v>
+        <v>0xf4400002,</v>
       </c>
       <c r="Y84">
         <f t="shared" si="42"/>
         <v>328</v>
       </c>
       <c r="Z84" t="str">
-        <f t="shared" si="24"/>
-        <v>0x00000150</v>
+        <f t="shared" si="27"/>
+        <v>0x00000154</v>
       </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26">
       <c r="A85" s="8"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
@@ -9962,11 +9973,11 @@
         <v>332</v>
       </c>
       <c r="Z85" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26">
       <c r="A86" s="1" t="s">
         <v>136</v>
       </c>
@@ -10058,11 +10069,11 @@
         <v>336</v>
       </c>
       <c r="Z86" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0x0000012C</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26">
       <c r="A87" s="5" t="s">
         <v>137</v>
       </c>
@@ -10149,11 +10160,11 @@
         <v>340</v>
       </c>
       <c r="Z87" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26">
       <c r="A88" s="5" t="s">
         <v>257</v>
       </c>
@@ -10243,11 +10254,11 @@
         <v>344</v>
       </c>
       <c r="Z88" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26">
       <c r="A89" s="8" t="s">
         <v>138</v>
       </c>
@@ -10337,11 +10348,11 @@
         <v>348</v>
       </c>
       <c r="Z89" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26">
       <c r="A90" s="1" t="s">
         <v>139</v>
       </c>
@@ -10431,11 +10442,11 @@
         <v>352</v>
       </c>
       <c r="Z90" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26">
       <c r="A91" s="5" t="s">
         <v>140</v>
       </c>
@@ -10525,11 +10536,11 @@
         <v>356</v>
       </c>
       <c r="Z91" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26">
       <c r="A92" s="5" t="s">
         <v>141</v>
       </c>
@@ -10619,11 +10630,11 @@
         <v>360</v>
       </c>
       <c r="Z92" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26">
       <c r="A93" s="8" t="s">
         <v>142</v>
       </c>
@@ -10713,11 +10724,11 @@
         <v>364</v>
       </c>
       <c r="Z93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26">
       <c r="A94" s="1" t="s">
         <v>143</v>
       </c>
@@ -10807,11 +10818,11 @@
         <v>368</v>
       </c>
       <c r="Z94" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26">
       <c r="A95" s="5" t="s">
         <v>144</v>
       </c>
@@ -10901,11 +10912,11 @@
         <v>372</v>
       </c>
       <c r="Z95" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26">
       <c r="A96" s="5" t="s">
         <v>146</v>
       </c>
@@ -10989,11 +11000,11 @@
         <v>376</v>
       </c>
       <c r="Z96" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26">
       <c r="A97" s="8" t="s">
         <v>147</v>
       </c>
@@ -11083,11 +11094,11 @@
         <v>380</v>
       </c>
       <c r="Z97" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26">
       <c r="A98" s="1" t="s">
         <v>148</v>
       </c>
@@ -11177,11 +11188,11 @@
         <v>384</v>
       </c>
       <c r="Z98" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26">
       <c r="A99" s="5" t="s">
         <v>257</v>
       </c>
@@ -11271,11 +11282,11 @@
         <v>388</v>
       </c>
       <c r="Z99" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:26">
       <c r="A100" s="5" t="s">
         <v>149</v>
       </c>
@@ -11294,8 +11305,8 @@
         <v>0x00000188</v>
       </c>
       <c r="F100" s="16">
-        <f>(D102-D101)/4</f>
-        <v>1</v>
+        <f>(D103-D101)/4</f>
+        <v>2</v>
       </c>
       <c r="G100" s="6" t="s">
         <v>105</v>
@@ -11367,11 +11378,11 @@
         <v>392</v>
       </c>
       <c r="Z100" t="str">
-        <f t="shared" si="24"/>
-        <v>0x00000190</v>
+        <f t="shared" si="27"/>
+        <v>0x00000194</v>
       </c>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:26">
       <c r="A101" s="8"/>
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
@@ -11455,11 +11466,11 @@
         <v>396</v>
       </c>
       <c r="Z101" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:26">
       <c r="A102" s="1" t="s">
         <v>150</v>
       </c>
@@ -11551,11 +11562,11 @@
         <v>400</v>
       </c>
       <c r="Z102" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0x00000170</v>
       </c>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:26">
       <c r="A103" s="5" t="s">
         <v>151</v>
       </c>
@@ -11645,11 +11656,11 @@
         <v>404</v>
       </c>
       <c r="Z103" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:26">
       <c r="A104" s="5" t="s">
         <v>153</v>
       </c>
@@ -11739,11 +11750,11 @@
         <v>408</v>
       </c>
       <c r="Z104" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:26">
       <c r="A105" s="8" t="s">
         <v>155</v>
       </c>
@@ -11833,11 +11844,11 @@
         <v>412</v>
       </c>
       <c r="Z105" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:26">
       <c r="A106" s="1" t="s">
         <v>157</v>
       </c>
@@ -11921,11 +11932,11 @@
         <v>416</v>
       </c>
       <c r="Z106" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:26">
       <c r="A107" s="5" t="s">
         <v>159</v>
       </c>
@@ -12015,11 +12026,11 @@
         <v>420</v>
       </c>
       <c r="Z107" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:26">
       <c r="A108" s="5" t="s">
         <v>160</v>
       </c>
@@ -12109,11 +12120,11 @@
         <v>424</v>
       </c>
       <c r="Z108" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:26">
       <c r="A109" s="8" t="s">
         <v>161</v>
       </c>
@@ -12203,11 +12214,11 @@
         <v>428</v>
       </c>
       <c r="Z109" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:26">
       <c r="A110" s="1" t="s">
         <v>163</v>
       </c>
@@ -12297,11 +12308,11 @@
         <v>432</v>
       </c>
       <c r="Z110" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="111" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:26">
       <c r="A111" s="5" t="s">
         <v>164</v>
       </c>
@@ -12391,11 +12402,11 @@
         <v>436</v>
       </c>
       <c r="Z111" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="112" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:26">
       <c r="A112" s="5" t="s">
         <v>165</v>
       </c>
@@ -12485,11 +12496,11 @@
         <v>440</v>
       </c>
       <c r="Z112" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="113" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:26">
       <c r="A113" s="8" t="s">
         <v>167</v>
       </c>
@@ -12579,11 +12590,11 @@
         <v>444</v>
       </c>
       <c r="Z113" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="114" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:26">
       <c r="A114" s="1" t="s">
         <v>168</v>
       </c>
@@ -12667,11 +12678,11 @@
         <v>448</v>
       </c>
       <c r="Z114" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="115" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:26">
       <c r="A115" s="5" t="s">
         <v>169</v>
       </c>
@@ -12761,11 +12772,11 @@
         <v>452</v>
       </c>
       <c r="Z115" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:26">
       <c r="A116" s="5" t="s">
         <v>170</v>
       </c>
@@ -12855,11 +12866,11 @@
         <v>456</v>
       </c>
       <c r="Z116" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="117" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:26">
       <c r="A117" s="8"/>
       <c r="B117" s="9"/>
       <c r="C117" s="9"/>
@@ -12943,11 +12954,11 @@
         <v>460</v>
       </c>
       <c r="Z117" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="118" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:26">
       <c r="A118" s="1" t="s">
         <v>257</v>
       </c>
@@ -13037,11 +13048,11 @@
         <v>464</v>
       </c>
       <c r="Z118" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="119" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:26">
       <c r="A119" s="5"/>
       <c r="B119" s="6"/>
       <c r="C119" s="6"/>
@@ -13125,11 +13136,11 @@
         <v>468</v>
       </c>
       <c r="Z119" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="120" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:26">
       <c r="A120" s="5" t="s">
         <v>171</v>
       </c>
@@ -13148,8 +13159,8 @@
         <v>0x000001D8</v>
       </c>
       <c r="F120" s="16">
-        <f>(D122-D121)/4</f>
-        <v>1</v>
+        <f>(D123-D121)/4</f>
+        <v>2</v>
       </c>
       <c r="G120" s="6" t="s">
         <v>105</v>
@@ -13166,7 +13177,7 @@
       </c>
       <c r="K120" s="7" t="str">
         <f>"0x"&amp;LOWER(IF(MID(DEC2HEX(F120,10),LEN(DEC2HEX(F120,10))-6,1)="F","1","0")&amp;MID(DEC2HEX(F120,10),LEN(DEC2HEX(F120,10))-4,5))</f>
-        <v>0x000001</v>
+        <v>0x000002</v>
       </c>
       <c r="L120" s="7"/>
       <c r="M120" s="7" t="str">
@@ -13179,7 +13190,7 @@
       </c>
       <c r="O120" s="7" t="str">
         <f>"00000"&amp;"00000000"&amp;HEX2BIN(MID(K120,3,99),8)</f>
-        <v>000000000000000000001</v>
+        <v>000000000000000000010</v>
       </c>
       <c r="P120" s="7" t="str">
         <f t="shared" si="34"/>
@@ -13198,11 +13209,11 @@
       </c>
       <c r="T120" s="7" t="str">
         <f t="shared" si="37"/>
-        <v>11110100010000000000000000000001</v>
+        <v>11110100010000000000000000000010</v>
       </c>
       <c r="U120" s="13" t="str">
         <f t="shared" si="47"/>
-        <v>0xf4400001</v>
+        <v>0xf4400002</v>
       </c>
       <c r="V120" s="7">
         <f t="shared" si="38"/>
@@ -13214,18 +13225,18 @@
       </c>
       <c r="X120" t="str">
         <f t="shared" si="40"/>
-        <v>0xf4400001,</v>
+        <v>0xf4400002,</v>
       </c>
       <c r="Y120">
         <f t="shared" si="42"/>
         <v>472</v>
       </c>
       <c r="Z120" t="str">
-        <f t="shared" ref="Z120:Z183" si="68">IF(ISBLANK(F120),"","0x"&amp;DEC2HEX(Y120+(F120*4)+4,8))</f>
-        <v>0x000001E0</v>
+        <f t="shared" si="27"/>
+        <v>0x000001E4</v>
       </c>
     </row>
-    <row r="121" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:26">
       <c r="A121" s="8"/>
       <c r="B121" s="9"/>
       <c r="C121" s="9"/>
@@ -13248,15 +13259,15 @@
         <v>514</v>
       </c>
       <c r="J121" s="10" t="str">
-        <f t="shared" ref="J121" si="69">MID(I121,1,FIND(",", I121)-1)</f>
+        <f t="shared" ref="J121" si="68">MID(I121,1,FIND(",", I121)-1)</f>
         <v>R31</v>
       </c>
       <c r="K121" s="10" t="str">
-        <f t="shared" ref="K121" si="70">TRIM(MID(I121,FIND(",",I121)+1,LEN(I121)-FIND(",",I121,FIND(",",I121)+1)))</f>
+        <f t="shared" ref="K121" si="69">TRIM(MID(I121,FIND(",",I121)+1,LEN(I121)-FIND(",",I121,FIND(",",I121)+1)))</f>
         <v>R31</v>
       </c>
       <c r="L121" s="10" t="str">
-        <f t="shared" ref="L121" si="71">TRIM(MID(I121,FIND(",",I121,FIND(",",I121)+1)+1,99))</f>
+        <f t="shared" ref="L121" si="70">TRIM(MID(I121,FIND(",",I121,FIND(",",I121)+1)+1,99))</f>
         <v>R31</v>
       </c>
       <c r="M121" s="10" t="str">
@@ -13268,24 +13279,24 @@
         <v>11111</v>
       </c>
       <c r="O121" s="10" t="str">
-        <f t="shared" ref="O121" si="72">IF(MID(K121,1,1)="#",DEC2BIN(MID(K121,2,99),8)&amp;"1",IF(MID(K121,1,1)="R",DEC2BIN(MID(K121,2,99),5)&amp;"0000",DEC2BIN(MID(K121,FIND("(",K121)+2,2),5)&amp;DEC2BIN(MID(K121,1,FIND("(",K121)-1),8)))</f>
+        <f t="shared" ref="O121" si="71">IF(MID(K121,1,1)="#",DEC2BIN(MID(K121,2,99),8)&amp;"1",IF(MID(K121,1,1)="R",DEC2BIN(MID(K121,2,99),5)&amp;"0000",DEC2BIN(MID(K121,FIND("(",K121)+2,2),5)&amp;DEC2BIN(MID(K121,1,FIND("(",K121)-1),8)))</f>
         <v>111110000</v>
       </c>
       <c r="P121" s="10" t="str">
-        <f t="shared" ref="P121" si="73">IFERROR(HEX2BIN(MID(H121,FIND(".",H121)+1,99),7),"")</f>
+        <f t="shared" ref="P121" si="72">IFERROR(HEX2BIN(MID(H121,FIND(".",H121)+1,99),7),"")</f>
         <v>0100000</v>
       </c>
       <c r="Q121" s="10" t="str">
-        <f t="shared" ref="Q121" si="74">IFERROR(DEC2BIN(MID(L121,2,2),5),"")</f>
+        <f t="shared" ref="Q121" si="73">IFERROR(DEC2BIN(MID(L121,2,2),5),"")</f>
         <v>11111</v>
       </c>
       <c r="R121" s="10">
-        <f t="shared" ref="R121" si="75">LEN(T121)</f>
+        <f t="shared" ref="R121" si="74">LEN(T121)</f>
         <v>32</v>
       </c>
       <c r="S121" s="10"/>
       <c r="T121" s="10" t="str">
-        <f t="shared" ref="T121" si="76">M121&amp;N121&amp;O121&amp;P121&amp;Q121</f>
+        <f t="shared" ref="T121" si="75">M121&amp;N121&amp;O121&amp;P121&amp;Q121</f>
         <v>01000111111111110000010000011111</v>
       </c>
       <c r="U121" s="11" t="str">
@@ -13309,11 +13320,11 @@
         <v>476</v>
       </c>
       <c r="Z121" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="122" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:26">
       <c r="A122" s="1" t="s">
         <v>172</v>
       </c>
@@ -13405,11 +13416,11 @@
         <v>480</v>
       </c>
       <c r="Z122" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="27"/>
         <v>0x000001B8</v>
       </c>
     </row>
-    <row r="123" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:26">
       <c r="A123" s="5" t="s">
         <v>173</v>
       </c>
@@ -13499,11 +13510,11 @@
         <v>484</v>
       </c>
       <c r="Z123" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="124" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:26">
       <c r="A124" s="5" t="s">
         <v>174</v>
       </c>
@@ -13593,11 +13604,11 @@
         <v>488</v>
       </c>
       <c r="Z124" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="125" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:26">
       <c r="A125" s="8" t="s">
         <v>176</v>
       </c>
@@ -13687,11 +13698,11 @@
         <v>492</v>
       </c>
       <c r="Z125" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:26">
       <c r="A126" s="1" t="s">
         <v>177</v>
       </c>
@@ -13775,11 +13786,11 @@
         <v>496</v>
       </c>
       <c r="Z126" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:26">
       <c r="A127" s="5" t="s">
         <v>178</v>
       </c>
@@ -13869,11 +13880,11 @@
         <v>500</v>
       </c>
       <c r="Z127" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:26">
       <c r="A128" s="5" t="s">
         <v>179</v>
       </c>
@@ -13963,11 +13974,11 @@
         <v>504</v>
       </c>
       <c r="Z128" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:26">
       <c r="A129" s="8" t="s">
         <v>180</v>
       </c>
@@ -14057,11 +14068,11 @@
         <v>508</v>
       </c>
       <c r="Z129" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
-    <row r="130" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:26">
       <c r="A130" s="1" t="s">
         <v>182</v>
       </c>
@@ -14151,11 +14162,11 @@
         <v>512</v>
       </c>
       <c r="Z130" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" ref="Z130:Z179" si="76">IF(ISBLANK(F130),"","0x"&amp;DEC2HEX(Y130+(F130*4)+4,8))</f>
         <v/>
       </c>
     </row>
-    <row r="131" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:26">
       <c r="A131" s="5" t="s">
         <v>183</v>
       </c>
@@ -14245,11 +14256,11 @@
         <v>516</v>
       </c>
       <c r="Z131" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="132" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:26">
       <c r="A132" s="5" t="s">
         <v>184</v>
       </c>
@@ -14339,11 +14350,11 @@
         <v>520</v>
       </c>
       <c r="Z132" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="133" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:26">
       <c r="A133" s="8" t="s">
         <v>186</v>
       </c>
@@ -14433,11 +14444,11 @@
         <v>524</v>
       </c>
       <c r="Z133" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="134" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:26">
       <c r="A134" s="1" t="s">
         <v>187</v>
       </c>
@@ -14521,11 +14532,11 @@
         <v>528</v>
       </c>
       <c r="Z134" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="135" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:26">
       <c r="A135" s="5" t="s">
         <v>188</v>
       </c>
@@ -14615,11 +14626,11 @@
         <v>532</v>
       </c>
       <c r="Z135" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="136" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:26">
       <c r="A136" s="5" t="s">
         <v>189</v>
       </c>
@@ -14709,11 +14720,11 @@
         <v>536</v>
       </c>
       <c r="Z136" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="137" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:26">
       <c r="A137" s="8"/>
       <c r="B137" s="9"/>
       <c r="C137" s="9"/>
@@ -14797,11 +14808,11 @@
         <v>540</v>
       </c>
       <c r="Z137" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="138" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:26">
       <c r="A138" s="1" t="s">
         <v>257</v>
       </c>
@@ -14891,11 +14902,11 @@
         <v>544</v>
       </c>
       <c r="Z138" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="139" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:26">
       <c r="A139" s="5"/>
       <c r="B139" s="6"/>
       <c r="C139" s="6"/>
@@ -14979,11 +14990,11 @@
         <v>548</v>
       </c>
       <c r="Z139" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="140" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:26">
       <c r="A140" s="5" t="s">
         <v>190</v>
       </c>
@@ -15002,8 +15013,8 @@
         <v>0x00000228</v>
       </c>
       <c r="F140" s="16">
-        <f>(D142-D141)/4</f>
-        <v>1</v>
+        <f>(D143-D141)/4</f>
+        <v>2</v>
       </c>
       <c r="G140" s="6" t="s">
         <v>105</v>
@@ -15020,7 +15031,7 @@
       </c>
       <c r="K140" s="7" t="str">
         <f>"0x"&amp;LOWER(IF(MID(DEC2HEX(F140,10),LEN(DEC2HEX(F140,10))-6,1)="F","1","0")&amp;MID(DEC2HEX(F140,10),LEN(DEC2HEX(F140,10))-4,5))</f>
-        <v>0x000001</v>
+        <v>0x000002</v>
       </c>
       <c r="L140" s="7"/>
       <c r="M140" s="7" t="str">
@@ -15033,7 +15044,7 @@
       </c>
       <c r="O140" s="7" t="str">
         <f>"00000"&amp;"00000000"&amp;HEX2BIN(MID(K140,3,99),8)</f>
-        <v>000000000000000000001</v>
+        <v>000000000000000000010</v>
       </c>
       <c r="P140" s="7" t="str">
         <f t="shared" ref="P140:P184" si="94">IFERROR(HEX2BIN(MID(H140,FIND(".",H140)+1,99),7),"")</f>
@@ -15052,11 +15063,11 @@
       </c>
       <c r="T140" s="7" t="str">
         <f t="shared" ref="T140:T184" si="97">M140&amp;N140&amp;O140&amp;P140&amp;Q140</f>
-        <v>11110100010000000000000000000001</v>
+        <v>11110100010000000000000000000010</v>
       </c>
       <c r="U140" s="13" t="str">
         <f t="shared" si="83"/>
-        <v>0xf4400001</v>
+        <v>0xf4400002</v>
       </c>
       <c r="V140" s="7">
         <f t="shared" si="78"/>
@@ -15068,18 +15079,18 @@
       </c>
       <c r="X140" t="str">
         <f t="shared" si="80"/>
-        <v>0xf4400001,</v>
+        <v>0xf4400002,</v>
       </c>
       <c r="Y140">
         <f t="shared" si="82"/>
         <v>552</v>
       </c>
       <c r="Z140" t="str">
-        <f t="shared" si="68"/>
-        <v>0x00000230</v>
+        <f t="shared" si="76"/>
+        <v>0x00000234</v>
       </c>
     </row>
-    <row r="141" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:26">
       <c r="A141" s="8"/>
       <c r="B141" s="9"/>
       <c r="C141" s="9"/>
@@ -15163,11 +15174,11 @@
         <v>556</v>
       </c>
       <c r="Z141" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="142" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:26">
       <c r="A142" s="1" t="s">
         <v>191</v>
       </c>
@@ -15259,11 +15270,11 @@
         <v>560</v>
       </c>
       <c r="Z142" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v>0x00000208</v>
       </c>
     </row>
-    <row r="143" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:26">
       <c r="A143" s="5" t="s">
         <v>192</v>
       </c>
@@ -15353,11 +15364,11 @@
         <v>564</v>
       </c>
       <c r="Z143" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="144" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:26">
       <c r="A144" s="5" t="s">
         <v>193</v>
       </c>
@@ -15447,11 +15458,11 @@
         <v>568</v>
       </c>
       <c r="Z144" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="145" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:26">
       <c r="A145" s="8" t="s">
         <v>195</v>
       </c>
@@ -15541,11 +15552,11 @@
         <v>572</v>
       </c>
       <c r="Z145" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="146" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:26">
       <c r="A146" s="1" t="s">
         <v>196</v>
       </c>
@@ -15629,11 +15640,11 @@
         <v>576</v>
       </c>
       <c r="Z146" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="147" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:26">
       <c r="A147" s="5"/>
       <c r="B147" s="6"/>
       <c r="C147" s="6"/>
@@ -15717,11 +15728,11 @@
         <v>580</v>
       </c>
       <c r="Z147" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="148" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:26">
       <c r="A148" s="5"/>
       <c r="B148" s="6"/>
       <c r="C148" s="6"/>
@@ -15805,11 +15816,11 @@
         <v>584</v>
       </c>
       <c r="Z148" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="149" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:26">
       <c r="A149" s="8"/>
       <c r="B149" s="9"/>
       <c r="C149" s="9"/>
@@ -15893,11 +15904,11 @@
         <v>588</v>
       </c>
       <c r="Z149" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="150" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:26">
       <c r="A150" s="1" t="s">
         <v>198</v>
       </c>
@@ -15987,11 +15998,11 @@
         <v>592</v>
       </c>
       <c r="Z150" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="151" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:26">
       <c r="A151" s="5" t="s">
         <v>199</v>
       </c>
@@ -16081,11 +16092,11 @@
         <v>596</v>
       </c>
       <c r="Z151" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="152" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:26">
       <c r="A152" s="5" t="s">
         <v>200</v>
       </c>
@@ -16175,11 +16186,11 @@
         <v>600</v>
       </c>
       <c r="Z152" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="153" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:26">
       <c r="A153" s="8" t="s">
         <v>201</v>
       </c>
@@ -16269,11 +16280,11 @@
         <v>604</v>
       </c>
       <c r="Z153" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="154" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:26">
       <c r="A154" s="1" t="s">
         <v>202</v>
       </c>
@@ -16363,11 +16374,11 @@
         <v>608</v>
       </c>
       <c r="Z154" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="155" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:26">
       <c r="A155" s="5"/>
       <c r="B155" s="6"/>
       <c r="C155" s="6"/>
@@ -16451,11 +16462,11 @@
         <v>612</v>
       </c>
       <c r="Z155" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="156" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:26">
       <c r="A156" s="5"/>
       <c r="B156" s="6"/>
       <c r="C156" s="6"/>
@@ -16539,11 +16550,11 @@
         <v>616</v>
       </c>
       <c r="Z156" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="157" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:26">
       <c r="A157" s="8"/>
       <c r="B157" s="9"/>
       <c r="C157" s="9"/>
@@ -16627,11 +16638,11 @@
         <v>620</v>
       </c>
       <c r="Z157" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="158" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:26">
       <c r="A158" s="1" t="s">
         <v>203</v>
       </c>
@@ -16721,11 +16732,11 @@
         <v>624</v>
       </c>
       <c r="Z158" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="159" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:26">
       <c r="A159" s="5" t="s">
         <v>204</v>
       </c>
@@ -16815,11 +16826,11 @@
         <v>628</v>
       </c>
       <c r="Z159" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="160" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:26">
       <c r="A160" s="5" t="s">
         <v>206</v>
       </c>
@@ -16903,11 +16914,11 @@
         <v>632</v>
       </c>
       <c r="Z160" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="161" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:26">
       <c r="A161" s="8" t="s">
         <v>208</v>
       </c>
@@ -16991,11 +17002,11 @@
         <v>636</v>
       </c>
       <c r="Z161" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="162" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:26">
       <c r="A162" s="1" t="s">
         <v>210</v>
       </c>
@@ -17085,11 +17096,11 @@
         <v>640</v>
       </c>
       <c r="Z162" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="163" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:26">
       <c r="A163" s="5" t="s">
         <v>212</v>
       </c>
@@ -17181,11 +17192,11 @@
         <v>644</v>
       </c>
       <c r="Z163" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v>0x0000029C</v>
       </c>
     </row>
-    <row r="164" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:26">
       <c r="A164" s="5" t="s">
         <v>215</v>
       </c>
@@ -17269,11 +17280,11 @@
         <v>648</v>
       </c>
       <c r="Z164" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="165" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:26">
       <c r="A165" s="8" t="s">
         <v>217</v>
       </c>
@@ -17357,11 +17368,11 @@
         <v>652</v>
       </c>
       <c r="Z165" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="166" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:26">
       <c r="A166" s="1" t="s">
         <v>218</v>
       </c>
@@ -17451,11 +17462,11 @@
         <v>656</v>
       </c>
       <c r="Z166" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="167" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:26">
       <c r="A167" s="5" t="s">
         <v>220</v>
       </c>
@@ -17545,11 +17556,11 @@
         <v>660</v>
       </c>
       <c r="Z167" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="168" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:26">
       <c r="A168" s="5" t="s">
         <v>222</v>
       </c>
@@ -17635,11 +17646,11 @@
         <v>664</v>
       </c>
       <c r="Z168" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="169" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:26">
       <c r="A169" s="8" t="s">
         <v>225</v>
       </c>
@@ -17729,11 +17740,11 @@
         <v>668</v>
       </c>
       <c r="Z169" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="170" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:26">
       <c r="A170" s="1" t="s">
         <v>226</v>
       </c>
@@ -17823,11 +17834,11 @@
         <v>672</v>
       </c>
       <c r="Z170" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="171" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:26">
       <c r="A171" s="5" t="s">
         <v>228</v>
       </c>
@@ -17917,11 +17928,11 @@
         <v>676</v>
       </c>
       <c r="Z171" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="172" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:26">
       <c r="A172" s="5" t="s">
         <v>230</v>
       </c>
@@ -18011,11 +18022,11 @@
         <v>680</v>
       </c>
       <c r="Z172" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="173" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:26">
       <c r="A173" s="8" t="s">
         <v>232</v>
       </c>
@@ -18105,11 +18116,11 @@
         <v>684</v>
       </c>
       <c r="Z173" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="174" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:26">
       <c r="A174" s="1" t="s">
         <v>234</v>
       </c>
@@ -18199,11 +18210,11 @@
         <v>688</v>
       </c>
       <c r="Z174" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="175" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:26">
       <c r="A175" s="5" t="s">
         <v>236</v>
       </c>
@@ -18293,11 +18304,11 @@
         <v>692</v>
       </c>
       <c r="Z175" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="176" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:26">
       <c r="A176" s="5" t="s">
         <v>238</v>
       </c>
@@ -18387,11 +18398,11 @@
         <v>696</v>
       </c>
       <c r="Z176" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="177" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:26">
       <c r="A177" s="8" t="s">
         <v>240</v>
       </c>
@@ -18481,11 +18492,11 @@
         <v>700</v>
       </c>
       <c r="Z177" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="178" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:26">
       <c r="A178" s="1" t="s">
         <v>242</v>
       </c>
@@ -18575,11 +18586,11 @@
         <v>704</v>
       </c>
       <c r="Z178" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="179" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:26">
       <c r="A179" s="5" t="s">
         <v>257</v>
       </c>
@@ -18669,11 +18680,11 @@
         <v>708</v>
       </c>
       <c r="Z179" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
     </row>
-    <row r="180" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:26">
       <c r="A180" s="5" t="s">
         <v>244</v>
       </c>
@@ -18765,11 +18776,11 @@
         <v>712</v>
       </c>
       <c r="Z180" t="str">
-        <f t="shared" si="68"/>
+        <f>IF(ISBLANK(F180),"","0x"&amp;DEC2HEX(Y180+(F180*4)+4,8))</f>
         <v>0x00000270</v>
       </c>
     </row>
-    <row r="181" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:26">
       <c r="A181" s="8" t="s">
         <v>246</v>
       </c>
@@ -18853,11 +18864,11 @@
         <v>716</v>
       </c>
       <c r="Z181" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" ref="Z181:Z185" si="122">IF(ISBLANK(F181),"","0x"&amp;DEC2HEX(Y181+(F181*4)+4,8))</f>
         <v/>
       </c>
     </row>
-    <row r="182" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:26">
       <c r="A182" s="1" t="s">
         <v>247</v>
       </c>
@@ -18941,11 +18952,11 @@
         <v>720</v>
       </c>
       <c r="Z182" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="122"/>
         <v/>
       </c>
     </row>
-    <row r="183" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:26">
       <c r="A183" s="5" t="s">
         <v>249</v>
       </c>
@@ -19035,11 +19046,11 @@
         <v>724</v>
       </c>
       <c r="Z183" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="122"/>
         <v/>
       </c>
     </row>
-    <row r="184" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:26">
       <c r="A184" s="5" t="s">
         <v>251</v>
       </c>
@@ -19129,14 +19140,20 @@
         <v>728</v>
       </c>
       <c r="Z184" t="str">
-        <f t="shared" ref="Z184:Z185" si="122">IF(ISBLANK(F184),"","0x"&amp;DEC2HEX(Y184+(F184*4)+4,8))</f>
+        <f t="shared" si="122"/>
         <v/>
       </c>
     </row>
-    <row r="185" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A185" s="8"/>
-      <c r="B185" s="9"/>
-      <c r="C185" s="9"/>
+    <row r="185" spans="1:26">
+      <c r="A185" s="8" t="s">
+        <v>522</v>
+      </c>
+      <c r="B185" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="C185" s="9" t="s">
+        <v>449</v>
+      </c>
       <c r="D185" s="17">
         <f t="shared" si="81"/>
         <v>732</v>
@@ -19145,83 +19162,82 @@
         <f t="shared" si="77"/>
         <v>0x000002DC</v>
       </c>
-      <c r="F185" s="17"/>
+      <c r="F185" s="17">
+        <f>(D181-(D185+4))/4</f>
+        <v>-5</v>
+      </c>
       <c r="G185" s="9" t="s">
-        <v>11</v>
+        <v>223</v>
       </c>
       <c r="H185" s="9" t="s">
-        <v>489</v>
-      </c>
-      <c r="I185" s="10" t="s">
-        <v>514</v>
+        <v>507</v>
+      </c>
+      <c r="I185" s="9" t="s">
+        <v>224</v>
       </c>
       <c r="J185" s="10" t="str">
         <f t="shared" ref="J185" si="123">MID(I185,1,FIND(",", I185)-1)</f>
         <v>R31</v>
       </c>
       <c r="K185" s="10" t="str">
-        <f t="shared" si="106"/>
-        <v>R31</v>
-      </c>
-      <c r="L185" s="10" t="str">
-        <f t="shared" si="107"/>
-        <v>R31</v>
-      </c>
+        <f>TRIM(MID(I185,FIND(",",I185)+1,99))</f>
+        <v>R00</v>
+      </c>
+      <c r="L185" s="10"/>
       <c r="M185" s="10" t="str">
-        <f>HEX2BIN(MID(H185,1,FIND(".",H185)-1),6)</f>
-        <v>010001</v>
+        <f t="shared" ref="M185" si="124">HEX2BIN(MID(H185,1,FIND(".",H185)-1),6)</f>
+        <v>011010</v>
       </c>
       <c r="N185" s="10" t="str">
-        <f t="shared" ref="N185" si="124">DEC2BIN(INT(MID(J185,2,2)),5)</f>
+        <f t="shared" ref="N185" si="125">DEC2BIN(INT(MID(J185,2,2)),5)</f>
         <v>11111</v>
       </c>
       <c r="O185" s="10" t="str">
-        <f t="shared" si="121"/>
-        <v>111110000</v>
+        <f t="shared" ref="O185" si="126">IF(MID(K185,1,1)="#",DEC2BIN(MID(K185,2,99),8)&amp;"1",IF(MID(K185,1,1)="R",DEC2BIN(MID(K185,2,99),5)&amp;"0000",DEC2BIN(MID(K185,FIND("(",K185)+2,2),5)&amp;DEC2BIN(MID(K185,1,FIND("(",K185)-1),8)))</f>
+        <v>000000000</v>
       </c>
       <c r="P185" s="10" t="str">
-        <f t="shared" ref="P185" si="125">IFERROR(HEX2BIN(MID(H185,FIND(".",H185)+1,99),7),"")</f>
-        <v>0100000</v>
-      </c>
-      <c r="Q185" s="10" t="str">
-        <f t="shared" si="95"/>
-        <v>11111</v>
+        <f t="shared" ref="P185" si="127">IFERROR(HEX2BIN(MID(H185,FIND(".",H185)+1,99),7),"")</f>
+        <v>0000000</v>
+      </c>
+      <c r="Q185" s="10" t="s">
+        <v>512</v>
       </c>
       <c r="R185" s="10">
-        <f t="shared" ref="R185" si="126">LEN(T185)</f>
+        <f t="shared" ref="R185" si="128">LEN(T185)</f>
         <v>32</v>
       </c>
       <c r="S185" s="10"/>
       <c r="T185" s="10" t="str">
-        <f t="shared" ref="T185" si="127">M185&amp;N185&amp;O185&amp;P185&amp;Q185</f>
-        <v>01000111111111110000010000011111</v>
+        <f t="shared" ref="T185" si="129">M185&amp;N185&amp;O185&amp;P185&amp;Q185</f>
+        <v>01101011111000000000000000000000</v>
       </c>
       <c r="U185" s="11" t="str">
-        <f t="shared" si="83"/>
-        <v>0x47ff041f</v>
+        <f t="shared" ref="U185" si="130">"0x"&amp;LOWER(BIN2HEX(MID(T185,1,8),2)&amp;BIN2HEX(MID(T185,9,8),2)&amp;BIN2HEX(MID(T185,17,8),2)&amp;BIN2HEX(MID(T185,25,8),2))</f>
+        <v>0x6be00000</v>
       </c>
       <c r="V185" s="7">
-        <f t="shared" si="78"/>
+        <f t="shared" ref="V185" si="131">LEN(U185)-2</f>
         <v>8</v>
       </c>
       <c r="W185" s="7" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" ref="W185" si="132">"0x"&amp;DEC2HEX(Y185,8)</f>
         <v>0x000002DC</v>
       </c>
-      <c r="X185" t="str">
-        <f>U185</f>
-        <v>0x47ff041f</v>
-      </c>
-      <c r="Y185">
+      <c r="X185" s="7" t="str">
+        <f t="shared" ref="X185" si="133">U185&amp;","</f>
+        <v>0x6be00000,</v>
+      </c>
+      <c r="Y185" s="7">
         <f t="shared" si="82"/>
         <v>732</v>
       </c>
       <c r="Z185" t="str">
         <f t="shared" si="122"/>
-        <v/>
+        <v>0x000002CC</v>
       </c>
     </row>
-    <row r="186" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:26">
       <c r="I186" s="18"/>
       <c r="J186" s="12"/>
       <c r="K186" s="18"/>
@@ -19230,22 +19246,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="R2:R5">
-    <cfRule type="cellIs" dxfId="5" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="32" operator="equal">
       <formula>32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R6:R185">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:W185">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S1:S185 S187:S1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="taken">
+  <conditionalFormatting sqref="S187:S1048576 S1:S185">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="taken">
       <formula>NOT(ISERROR(SEARCH("taken",S1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19255,24 +19271,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>